<commit_message>
update: melhora drastica e novas atualizações
</commit_message>
<xml_diff>
--- a/dados_coleta_plantas.xlsx
+++ b/dados_coleta_plantas.xlsx
@@ -551,7 +551,11 @@
           <t>6944</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -661,7 +665,11 @@
           <t>8031</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>'084S</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
           <t>31</t>
@@ -787,7 +795,11 @@
           <t>1691</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>]</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
           <t>21</t>
@@ -928,11 +940,7 @@
           <t>255</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>11/02/2000</t>
-        </is>
-      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
           <t>11</t>

</xml_diff>

<commit_message>
update: criação da lista de palavras ignoradas
</commit_message>
<xml_diff>
--- a/dados_coleta_plantas.xlsx
+++ b/dados_coleta_plantas.xlsx
@@ -536,29 +536,24 @@
           <t>APOCYNACEAE</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Secondary
-forest
-Occasional
-Tree
-fruits warty.
-D.C .</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>6944</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>1991</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -652,24 +647,9 @@
           <t>MELIACEAE</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Rio
-Muru,
-Seringal
-Lancha</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>8031</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>'084S</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
           <t>31</t>
@@ -785,34 +765,22 @@
           <t>crhysobalanaceae</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Kos</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1691</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>]</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>81</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1989</t>
+          <t>1990</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -928,18 +896,8 @@
           <t>HELICONIACEAE</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>com flores alaranjada
-N.V
-Rivero, L.S.com</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>255</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
update: começando a pegar os coletores
</commit_message>
<xml_diff>
--- a/dados_coleta_plantas.xlsx
+++ b/dados_coleta_plantas.xlsx
@@ -536,8 +536,16 @@
           <t>APOCYNACEAE</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>LiRE m Daly</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>69058</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
@@ -647,8 +655,16 @@
           <t>MELIACEAE</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>preto Oliveira; A RS</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>8031</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
@@ -766,8 +782,16 @@
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>et al.</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
           <t>10</t>
@@ -897,7 +921,11 @@
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>90957</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>

</xml_diff>